<commit_message>
Members updated, Update ALUMNI_DATA to update Page
</commit_message>
<xml_diff>
--- a/Alumni_Detail/Alumni Detail.xlsx
+++ b/Alumni_Detail/Alumni Detail.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prana\Desktop\Robocon\Website\Official-Website-2022\Alumni_Detail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC79328-1D39-4067-99F8-0B6D821070C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB39479-B4AE-4B8B-A609-90B91339E166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4404" yWindow="612" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2023" sheetId="5" r:id="rId1"/>
-    <sheet name="2022" sheetId="1" r:id="rId2"/>
-    <sheet name="2020" sheetId="2" r:id="rId3"/>
-    <sheet name="2019" sheetId="3" r:id="rId4"/>
-    <sheet name="2018" sheetId="4" r:id="rId5"/>
-    <sheet name="2015" sheetId="6" r:id="rId6"/>
+    <sheet name="&quot;2023&quot;" sheetId="5" r:id="rId1"/>
+    <sheet name="&quot;2022&quot;" sheetId="1" r:id="rId2"/>
+    <sheet name="&quot;2020&quot;" sheetId="2" r:id="rId3"/>
+    <sheet name="&quot;2019&quot;" sheetId="3" r:id="rId4"/>
+    <sheet name="&quot;2018&quot;" sheetId="4" r:id="rId5"/>
+    <sheet name="&quot;2015&quot;" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Team Lead</t>
   </si>
   <si>
-    <t>Team Lead"A playground to experiment, experience and excel for the talented and dedicated."</t>
-  </si>
-  <si>
     <t>"The three years of my experience at Robocon was the most accurate sample of the techno-corpotate work life outside the university walls. The time and effort I dedicated to the team led me to upgrade and polish my self as an engineer, a team player and a leader."</t>
   </si>
   <si>
@@ -200,13 +197,22 @@
     <t>https://www.linkedin.com/in/satyapalsinh-gohil-82b409181/</t>
   </si>
   <si>
-    <t>"Amidst the whirl of gears and the hum of motors, the fondest memory of the collective exhilaration of successfully unveiling, through seamless teamwork and boundless camaraderie, our meticulously designed and tirelessly built robot during the competition—a moment where our dedication, collaboration, and shared passion culminated in a triumphant symphony of innovation."</t>
-  </si>
-  <si>
     <t>Satyapalsinh Gohil is currently pursuing MS in Robotics from New York University (NYU).</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>"A playground to experiment, experience and excel for the talented and dedicated."</t>
+  </si>
+  <si>
+    <t>"The best memories in the club for me was the train journey to the competition and the shopping before that."</t>
+  </si>
+  <si>
+    <t>Abhishek Devidas Pawar currently works at NEOGOV as QA Analyst.</t>
+  </si>
+  <si>
+    <t>""Amidst the whirl of gears and the hum of motors, the fondest memory of the collective exhilaration of successfully unveiling, through seamless teamwork and boundless camaraderie, our meticulously designed and tirelessly built robot— a moment where our dedication, collaboration, and shared passion culminated in a triumphant symphony of innovation."</t>
   </si>
 </sst>
 </file>
@@ -545,7 +551,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F2"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,10 +624,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,13 +679,13 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -688,50 +694,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3" t="s">
-        <v>57</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{01B12A5D-2C30-4AA5-85BA-F7D020311410}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8EDB73-EA1B-4581-AFA5-A644AF95B3A3}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A3" sqref="A3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -779,24 +753,54 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
         <v>21</v>
       </c>
       <c r="I2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{8F0F7042-5787-487B-AC11-38B7C2E7F682}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{D2B8F94A-B6F5-425E-BD3A-3AD0D317BFBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -807,7 +811,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,45 +853,54 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
       <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>49</v>
+      <c r="I3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -942,31 +955,31 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>34</v>
-      </c>
-      <c r="I2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -981,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85BE488-F1F3-41F4-934B-A3D72266D4D4}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1018,7 +1031,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -1027,51 +1040,51 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>38</v>
-      </c>
-      <c r="I2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
       </c>
       <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" t="s">
         <v>42</v>
       </c>
-      <c r="E3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>43</v>
-      </c>
-      <c r="I3" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Only active social media will open a new page
</commit_message>
<xml_diff>
--- a/Alumni_Detail/Alumni Detail.xlsx
+++ b/Alumni_Detail/Alumni Detail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prana\Desktop\Robocon\Website\Official-Website-2022\Alumni_Detail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB39479-B4AE-4B8B-A609-90B91339E166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC203043-7A8E-4D40-9B60-D168BB759EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4404" yWindow="612" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4404" yWindow="612" windowWidth="17280" windowHeight="8880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="&quot;2023&quot;" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -198,9 +198,6 @@
   </si>
   <si>
     <t>Satyapalsinh Gohil is currently pursuing MS in Robotics from New York University (NYU).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
   </si>
   <si>
     <t>"A playground to experiment, experience and excel for the talented and dedicated."</t>
@@ -626,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,14 +675,8 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>56</v>
-      </c>
       <c r="F2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>56</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -705,7 +696,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:I3"/>
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,14 +743,8 @@
       <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
-        <v>56</v>
-      </c>
       <c r="F2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G2" t="s">
-        <v>56</v>
       </c>
       <c r="H2" t="s">
         <v>21</v>
@@ -781,17 +766,11 @@
       <c r="D3" t="s">
         <v>53</v>
       </c>
-      <c r="E3" t="s">
-        <v>56</v>
-      </c>
       <c r="F3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I3" t="s">
         <v>55</v>
@@ -811,7 +790,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -856,16 +835,13 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="G2" t="s">
-        <v>56</v>
       </c>
       <c r="H2" t="s">
         <v>26</v>
@@ -887,9 +863,6 @@
       <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
-        <v>56</v>
-      </c>
       <c r="F3" s="1" t="s">
         <v>47</v>
       </c>
@@ -897,10 +870,10 @@
         <v>48</v>
       </c>
       <c r="H3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" t="s">
         <v>58</v>
-      </c>
-      <c r="I3" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -919,7 +892,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -966,14 +939,8 @@
       <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s">
-        <v>56</v>
-      </c>
       <c r="F2" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="G2" t="s">
-        <v>56</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -994,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85BE488-F1F3-41F4-934B-A3D72266D4D4}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1042,14 +1009,8 @@
       <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" t="s">
-        <v>56</v>
-      </c>
       <c r="F2" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="G2" t="s">
-        <v>56</v>
       </c>
       <c r="H2" t="s">
         <v>37</v>
@@ -1071,15 +1032,10 @@
       <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="E3" t="s">
-        <v>56</v>
-      </c>
       <c r="F3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="G3" s="1"/>
       <c r="H3" t="s">
         <v>42</v>
       </c>
@@ -1091,7 +1047,6 @@
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{81407BFD-91A6-44C6-9B6F-09D73EC75686}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{D6410CEC-E55E-4B48-888F-CE93D4763867}"/>
-    <hyperlink ref="G3" r:id="rId3" display="https://www.instagram.com/sorabhgandhi/" xr:uid="{A1427D94-B294-4733-9B07-0A8D1C9D8D22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>